<commit_message>
Add Pickens County data from DHEC and SC Stats
</commit_message>
<xml_diff>
--- a/southCarolina.xlsx
+++ b/southCarolina.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/ttn-clemson-covid-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E655F0-D524-CE46-9689-E09E2A9BC3E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F234B1-4AAE-C746-8BDA-34D267D559A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTP CSV" sheetId="3" r:id="rId1"/>
     <sheet name="Daily Data" sheetId="1" r:id="rId2"/>
     <sheet name="Weekly Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Statistics" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Daily Data'!$E$2:$E$244</definedName>
@@ -804,63 +805,11 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -20454,7 +20403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -32934,7 +32883,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A2:A244">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),7)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32949,8 +32898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:P1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -33508,4 +33457,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CEBAE4-8D4D-7847-89C2-8E60DAA1E98A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>